<commit_message>
declare properties of GADPerson, GADStudent, GADSGA and GADFacStaff
</commit_message>
<xml_diff>
--- a/detail fields.xlsx
+++ b/detail fields.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/appdev/Desktop/AppDev/NewDB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/appdev/Documents/DB-iOS/NewDB-iOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="460" windowWidth="25600" windowHeight="14020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="13940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="77">
   <si>
     <t>SGA</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>not off campus study</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -571,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -947,6 +950,12 @@
       <c r="A27" t="s">
         <v>20</v>
       </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -1022,20 +1031,32 @@
       <c r="A33" t="s">
         <v>41</v>
       </c>
+      <c r="B33" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>42</v>
       </c>
+      <c r="B34" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>15</v>
       </c>
+      <c r="B35" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>43</v>
+      </c>
+      <c r="B36" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>